<commit_message>
Fixed unit in excel table
</commit_message>
<xml_diff>
--- a/Reports/FP-Calculation.xlsx
+++ b/Reports/FP-Calculation.xlsx
@@ -5,27 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Desktop\DHBW\eventlab-doc\Software Requirements Specification\Use Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Desktop\DHBW\eventlab-doc\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB4259B-709A-47F5-8F8A-7FCA6B30470E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E97BBB-C3D5-4209-93F8-77FF7B4AA262}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Tabellenblatt1!$B$12:$B$14</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Tabellenblatt1!$B$3:$B$6</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Tabellenblatt1!$C$12:$C$14</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Tabellenblatt1!$C$3:$C$6</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Tabellenblatt1!$B$12:$B$14</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Tabellenblatt1!$B$3:$B$6</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Tabellenblatt1!$C$12:$C$14</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Tabellenblatt1!$C$2</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Tabellenblatt1!$C$3:$C$6</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -82,13 +71,13 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Average hours per function point</t>
-  </si>
-  <si>
     <t>Future use cases</t>
   </si>
   <si>
     <t>Total remaining effort</t>
+  </si>
+  <si>
+    <t>Average minutes per function point</t>
   </si>
 </sst>
 </file>
@@ -1833,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1933,7 +1922,7 @@
     </row>
     <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" s="21">
         <f>B7/C7</f>
@@ -1946,7 +1935,7 @@
     </row>
     <row r="11" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>12</v>
@@ -2020,7 +2009,7 @@
     </row>
     <row r="17" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="18">
         <f>SUM(B12:B16)</f>

</xml_diff>

<commit_message>
Added actual time spend for UC
</commit_message>
<xml_diff>
--- a/Reports/FP-Calculation.xlsx
+++ b/Reports/FP-Calculation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D070369\OneDrive - SAP SE\Desktop\DHBW\Semester 3\SE\project\eventlab-doc\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d070473\Git\eventlab-doc\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{79E97BBB-C3D5-4209-93F8-77FF7B4AA262}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1793B5F3-AD34-4F34-A69F-0302209D56DD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9592A303-1047-4FD3-947C-9F50E3F07F00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Function Points</t>
   </si>
@@ -87,7 +87,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -149,8 +149,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +194,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -203,11 +223,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -234,13 +251,19 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="20% - Accent4" xfId="3" builtinId="42"/>
-    <cellStyle name="20% - Accent5" xfId="4" builtinId="46"/>
-    <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
+    <cellStyle name="20 % - Akzent4" xfId="3" builtinId="42"/>
+    <cellStyle name="20 % - Akzent5" xfId="4" builtinId="46"/>
+    <cellStyle name="40 % - Akzent1" xfId="2" builtinId="31"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -264,7 +287,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -350,7 +373,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Finished use cases</c:v>
+            <c:v>First Semester use cases</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -399,7 +422,7 @@
             <c:numRef>
               <c:f>Tabellenblatt1!$C$3:$C$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>131.76</c:v>
@@ -427,7 +450,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Future use cases (estimation)</c:v>
+            <c:v>Second Semester use cases (estimation)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -506,6 +529,89 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000009-1CCA-49D4-A941-9525FD79B4F7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Second Semester use cases (actual)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabellenblatt1!$D$12:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1103</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1361</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>955</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1033</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>799</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabellenblatt1!$C$12:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.399999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-850B-4E26-AD15-AC64AED4C3B9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -576,8 +682,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.21892717632020878"/>
-              <c:y val="0.91808948298488879"/>
+              <c:x val="1.2852034180141636E-2"/>
+              <c:y val="0.91175981708418741"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -740,7 +846,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -795,10 +901,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.63247620176294805"/>
-          <c:y val="0.91991669068552495"/>
-          <c:w val="0.36752386940441023"/>
-          <c:h val="5.7071124403461973E-2"/>
+          <c:x val="0.20741277795827581"/>
+          <c:y val="0.91991674959132363"/>
+          <c:w val="0.79258722204172416"/>
+          <c:h val="5.7067963424567769E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1428,16 +1534,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>949569</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>199476</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>23444</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>2778369</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>87923</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2024062</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1524,7 +1630,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1822,252 +1928,272 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.21875" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="62" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>2707</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="21">
         <v>131.76</v>
       </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="11">
         <v>2271</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="21">
         <v>128.26</v>
       </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>2413</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="21">
         <v>47.12</v>
       </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <v>1749</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="21">
         <v>36.58</v>
       </c>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <f>SUM(B3:B6)</f>
         <v>9140</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <f>SUM(C3:C6)</f>
         <v>343.71999999999997</v>
       </c>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="20">
         <f>B7/C7</f>
         <v>26.591411614104505</v>
       </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
+      <c r="D11" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="15">
         <f>1/0.0386*C12</f>
         <v>1424.8704663212436</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="16">
         <v>55</v>
       </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
+      <c r="D12" s="22">
+        <v>1103</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="15">
         <f t="shared" ref="B13:B16" si="0">1/0.0386*C13</f>
         <v>580.82901554404145</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="16">
         <v>22.42</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
+      <c r="D13" s="22">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="15">
         <f t="shared" si="0"/>
         <v>1865.2849740932643</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="16">
         <v>72</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
+      <c r="D14" s="22">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="15">
         <f t="shared" si="0"/>
         <v>550.25906735751289</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="16">
         <v>21.24</v>
       </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
+      <c r="D15" s="23">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="15">
         <f t="shared" si="0"/>
         <v>528.49740932642487</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="16">
         <v>20.399999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
+      <c r="D16" s="22">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="17">
         <f>SUM(B12:B16)</f>
         <v>4949.7409326424868</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="13">
         <f>SUM(C12:C16)</f>
         <v>191.06000000000003</v>
       </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B18" s="13"/>
-    </row>
-    <row r="19" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:13" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:13" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:13" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
-    </row>
-    <row r="26" spans="1:13" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:13" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:13" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:13" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:13" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:13" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:13" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D95" s="7"/>
-      <c r="E95" s="7"/>
-    </row>
-    <row r="96" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D96" s="6"/>
-    </row>
-    <row r="97" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D97" s="6"/>
-    </row>
-    <row r="98" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D98" s="6"/>
+      <c r="D17" s="24">
+        <f>SUM(D12:D16)</f>
+        <v>5251</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B18" s="12"/>
+    </row>
+    <row r="19" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:13" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:13" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:13" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="1:13" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:13" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:13" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:13" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:13" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:13" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:13" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="95" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+    </row>
+    <row r="96" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D96" s="5"/>
+    </row>
+    <row r="97" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D97" s="5"/>
+    </row>
+    <row r="98" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D98" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>